<commit_message>
Added Flights Page and made changes to other files
</commit_message>
<xml_diff>
--- a/EaseMyTrip/src/test/resources/objectrepository/FlightDetails.xlsx
+++ b/EaseMyTrip/src/test/resources/objectrepository/FlightDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savithaselvaraj/git/EaseMyTrip/EaseMyTrip/src/test/resources/objectrepository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2566AEF2-2B7B-6540-8D8C-B8E002A26774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16DADD6-8AE6-5448-8113-1B114997F1B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15520" activeTab="1" xr2:uid="{D3F5C180-57E5-144C-A0BD-109FA2060A8F}"/>
+    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15520" xr2:uid="{D3F5C180-57E5-144C-A0BD-109FA2060A8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Flight Name</t>
   </si>
@@ -46,24 +46,12 @@
     <t>Chennai</t>
   </si>
   <si>
-    <t>APR</t>
-  </si>
-  <si>
     <t>FROM</t>
   </si>
   <si>
     <t>TO</t>
   </si>
   <si>
-    <t>MONTH</t>
-  </si>
-  <si>
-    <t>YEAR</t>
-  </si>
-  <si>
-    <t>DAY</t>
-  </si>
-  <si>
     <t>ADULTS</t>
   </si>
   <si>
@@ -92,6 +80,12 @@
   </si>
   <si>
     <t>Price</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>12/12/2022</t>
   </si>
 </sst>
 </file>
@@ -450,50 +444,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4524B536-E955-7442-B229-9C233E6B3060}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="2" max="3" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -501,25 +487,19 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
-        <v>2022</v>
-      </c>
-      <c r="E2" s="1">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -532,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EC1D6A-88F4-5749-9660-86CE9BB428A8}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -540,6 +520,9 @@
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -547,13 +530,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Integrated reading and writing from/to excel sheets respectively
</commit_message>
<xml_diff>
--- a/EaseMyTrip/src/test/resources/objectrepository/FlightDetails.xlsx
+++ b/EaseMyTrip/src/test/resources/objectrepository/FlightDetails.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savithaselvaraj/eclipse-workspace/ExcelSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/savithaselvaraj/git/EaseMyTrip/EaseMyTrip/src/test/resources/objectrepository/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195ADED3-C76B-8147-ADF0-A9D74E814A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6C40D6-5C43-0840-AE4D-BFA8392E2620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15520" xr2:uid="{D3F5C180-57E5-144C-A0BD-109FA2060A8F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" activeTab="1" xr2:uid="{D3F5C180-57E5-144C-A0BD-109FA2060A8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Search" sheetId="1" r:id="rId1"/>
+    <sheet name="Flights" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="49">
   <si>
     <t>From</t>
   </si>
@@ -46,58 +46,142 @@
     <t>Date of Travel</t>
   </si>
   <si>
-    <t>Month of Travel</t>
-  </si>
-  <si>
-    <t>Start Time</t>
-  </si>
-  <si>
-    <t>Flight Name</t>
-  </si>
-  <si>
-    <t>MUM</t>
-  </si>
-  <si>
-    <t>MAA</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>Adults</t>
-  </si>
-  <si>
-    <t>Go First</t>
-  </si>
-  <si>
-    <t>18:40</t>
-  </si>
-  <si>
-    <t>Spicejet</t>
-  </si>
-  <si>
-    <t>20:25</t>
-  </si>
-  <si>
-    <t>AirAsia</t>
-  </si>
-  <si>
-    <t>20:10</t>
-  </si>
-  <si>
-    <t>IndiGo</t>
-  </si>
-  <si>
-    <t>20:00</t>
+    <t>3/14/2022</t>
+  </si>
+  <si>
+    <t>TravelClass</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Infant</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Prem.Economy</t>
+  </si>
+  <si>
+    <t>Flights</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Departure Time</t>
+  </si>
+  <si>
+    <t>Arrival time</t>
+  </si>
+  <si>
+    <t>Vistara</t>
+  </si>
+  <si>
+    <t>10:25</t>
+  </si>
+  <si>
+    <t>16:20</t>
+  </si>
+  <si>
+    <t>58,823</t>
+  </si>
+  <si>
+    <t>15:45</t>
+  </si>
+  <si>
+    <t>22:45</t>
+  </si>
+  <si>
+    <t>14:40</t>
+  </si>
+  <si>
+    <t>11:55</t>
+  </si>
+  <si>
+    <t>20:15</t>
+  </si>
+  <si>
+    <t>06:30</t>
+  </si>
+  <si>
+    <t>06:00</t>
+  </si>
+  <si>
+    <t>09:55</t>
+  </si>
+  <si>
+    <t>21:55</t>
+  </si>
+  <si>
+    <t>20:55</t>
+  </si>
+  <si>
+    <t>19:45</t>
   </si>
   <si>
     <t>18:30</t>
   </si>
   <si>
-    <t>Multi-Airline</t>
-  </si>
-  <si>
-    <t>19:25</t>
+    <t>17:35</t>
+  </si>
+  <si>
+    <t>08:45</t>
+  </si>
+  <si>
+    <t>65,981</t>
+  </si>
+  <si>
+    <t>11:30</t>
+  </si>
+  <si>
+    <t>85,762</t>
+  </si>
+  <si>
+    <t>12:15</t>
+  </si>
+  <si>
+    <t>90,462</t>
+  </si>
+  <si>
+    <t>10:45</t>
+  </si>
+  <si>
+    <t>90,907</t>
+  </si>
+  <si>
+    <t>13:20</t>
+  </si>
+  <si>
+    <t>94,077</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>97,842</t>
+  </si>
+  <si>
+    <t>19:10</t>
+  </si>
+  <si>
+    <t>07:00</t>
+  </si>
+  <si>
+    <t>98,402</t>
+  </si>
+  <si>
+    <t>09:05</t>
+  </si>
+  <si>
+    <t>98,962</t>
   </si>
 </sst>
 </file>
@@ -134,8 +218,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,19 +535,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4524B536-E955-7442-B229-9C233E6B3060}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="13.6640625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="11.1640625" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="16.1640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.5" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,27 +560,39 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2">
-        <v>25</v>
+      <c r="D2" t="s">
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -503,150 +602,661 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48EC1D6A-88F4-5749-9660-86CE9BB428A8}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" customWidth="true" width="16.33203125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="17.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="B33" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="s">
+        <v>42</v>
+      </c>
+      <c r="C34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45" t="s">
+        <v>42</v>
+      </c>
+      <c r="C45" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>